<commit_message>
updated test trial counterbalance
</commit_message>
<xml_diff>
--- a/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
+++ b/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Documents/CMCM Lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065332CE-C01C-204F-8726-0CC1363CEC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED3E414-E416-E24B-AAAC-4F654F90B0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="164">
   <si>
     <t>curvilinear</t>
   </si>
@@ -1138,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EB3C47-5A75-7B42-A854-C31509C645B3}">
   <dimension ref="A1:AS56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1300,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>46</v>
@@ -1385,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>30</v>
@@ -1470,7 +1470,7 @@
         <v>46</v>
       </c>
       <c r="G5" s="52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>33</v>
@@ -1546,7 +1546,7 @@
         <v>46</v>
       </c>
       <c r="G6" s="52">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M6" t="s">
         <v>34</v>
@@ -1622,7 +1622,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="52">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="26"/>
@@ -1661,7 +1661,7 @@
         <v>30</v>
       </c>
       <c r="G8" s="53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1741,7 +1741,7 @@
         <v>46</v>
       </c>
       <c r="G10" s="53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M10" t="s">
         <v>142</v>
@@ -1790,7 +1790,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M11" t="s">
         <v>27</v>
@@ -1848,7 +1848,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="53">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>28</v>
@@ -1907,7 +1907,7 @@
         <v>46</v>
       </c>
       <c r="G13" s="53">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>28</v>
@@ -1960,7 +1960,7 @@
         <v>46</v>
       </c>
       <c r="G14" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="20" t="s">
         <v>29</v>
@@ -1984,6 +1984,7 @@
       <c r="U14" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="X14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
@@ -2041,11 +2042,9 @@
         <v>157</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="X15" s="4" t="s">
         <v>159</v>
       </c>
+      <c r="X15" s="26"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="26"/>
       <c r="AK15" s="26"/>
@@ -2078,7 +2077,7 @@
         <v>30</v>
       </c>
       <c r="G16" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M16" s="55" t="s">
         <v>30</v>
@@ -2108,9 +2107,7 @@
       <c r="W16" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="X16" s="18" t="s">
-        <v>90</v>
-      </c>
+      <c r="X16" s="26"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="26"/>
@@ -2143,7 +2140,7 @@
         <v>46</v>
       </c>
       <c r="G17" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M17" s="55" t="s">
         <v>30</v>
@@ -2168,17 +2165,12 @@
         <v>32</v>
       </c>
       <c r="V17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="W17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="W17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="X17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
+      <c r="X17" s="26"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
@@ -2211,7 +2203,7 @@
         <v>46</v>
       </c>
       <c r="G18" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K18" t="s">
         <v>161</v>
@@ -2235,18 +2227,13 @@
       <c r="S18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="U18" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="V18" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="W18" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="X18" s="18" t="s">
-        <v>90</v>
-      </c>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
@@ -2279,7 +2266,7 @@
         <v>30</v>
       </c>
       <c r="G19" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M19" s="18" t="s">
         <v>125</v>
@@ -2300,18 +2287,13 @@
       <c r="S19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="U19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="V19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="W19" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="X19" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="U19" t="s">
+        <v>103</v>
+      </c>
+      <c r="X19" s="26"/>
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
@@ -2347,18 +2329,14 @@
         <v>1</v>
       </c>
       <c r="P20" s="2"/>
-      <c r="U20" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="V20" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="W20" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="X20" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="X20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
@@ -2391,21 +2369,16 @@
         <v>46</v>
       </c>
       <c r="G21" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P21" s="2"/>
-      <c r="U21" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="V21" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="W21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="X21" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="X21" s="26"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
@@ -2438,7 +2411,7 @@
         <v>46</v>
       </c>
       <c r="G22" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M22" t="s">
         <v>142</v>
@@ -2485,7 +2458,7 @@
         <v>30</v>
       </c>
       <c r="G23" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M23" t="s">
         <v>27</v>
@@ -2505,9 +2478,6 @@
       </c>
       <c r="S23" t="s">
         <v>26</v>
-      </c>
-      <c r="U23" t="s">
-        <v>103</v>
       </c>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
@@ -2541,7 +2511,7 @@
         <v>30</v>
       </c>
       <c r="G24" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>28</v>
@@ -2561,10 +2531,6 @@
       </c>
       <c r="S24" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
@@ -2598,7 +2564,7 @@
         <v>46</v>
       </c>
       <c r="G25" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>28</v>
@@ -2618,9 +2584,6 @@
       </c>
       <c r="S25" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="V25" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="2"/>
@@ -2672,7 +2635,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="26"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="26"/>
       <c r="M27" s="20" t="s">
         <v>29</v>
       </c>
@@ -2706,10 +2669,10 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="2"/>
       <c r="M28" s="55" t="s">
         <v>30</v>
@@ -2743,6 +2706,12 @@
       <c r="AS28" s="2"/>
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
       <c r="M29" s="55" t="s">
         <v>30</v>
       </c>
@@ -2954,6 +2923,7 @@
       <c r="F56" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
edits to counterbalance & script
</commit_message>
<xml_diff>
--- a/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
+++ b/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8657D5F5-A164-D149-9A44-5FE1D012E7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0FAF40-5EDF-104F-BC69-162C26A7D579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="179">
   <si>
     <t>curvilinear</t>
   </si>
@@ -557,6 +557,21 @@
   </si>
   <si>
     <t>Test Q Order Lengend</t>
+  </si>
+  <si>
+    <t>Left Side</t>
+  </si>
+  <si>
+    <t>Right Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In test trial, the video on the left side will always be played first </t>
+  </si>
+  <si>
+    <t>Test Event Order</t>
+  </si>
+  <si>
+    <t>Test Event Legend</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1268,7 @@
   <dimension ref="A1:AU56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1266,14 +1281,14 @@
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="9" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" customWidth="1"/>
     <col min="15" max="15" width="18.1640625" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
     <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="21" max="21" width="19.83203125" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
     <col min="24" max="24" width="10.33203125" customWidth="1"/>
     <col min="27" max="27" width="8.6640625" customWidth="1"/>
     <col min="28" max="28" width="11.33203125" customWidth="1"/>
@@ -1304,7 +1319,7 @@
         <v>82</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>165</v>
@@ -1314,6 +1329,9 @@
       </c>
       <c r="O1" s="3" t="s">
         <v>147</v>
+      </c>
+      <c r="T1" t="s">
+        <v>161</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>148</v>
@@ -1352,8 +1370,8 @@
       <c r="G2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="52">
-        <v>1</v>
+      <c r="H2" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="I2" s="52" t="s">
         <v>166</v>
@@ -1434,8 +1452,8 @@
       <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="52">
-        <v>1</v>
+      <c r="H3" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="I3" s="52" t="s">
         <v>166</v>
@@ -1525,8 +1543,8 @@
       <c r="G4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="52">
-        <v>1</v>
+      <c r="H4" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="I4" s="52" t="s">
         <v>167</v>
@@ -1616,8 +1634,8 @@
       <c r="G5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="52">
-        <v>1</v>
+      <c r="H5" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="I5" s="52" t="s">
         <v>167</v>
@@ -1698,8 +1716,8 @@
       <c r="G6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="52">
-        <v>2</v>
+      <c r="H6" s="52" t="s">
+        <v>43</v>
       </c>
       <c r="I6" s="52" t="s">
         <v>167</v>
@@ -1780,8 +1798,8 @@
       <c r="G7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="52">
-        <v>2</v>
+      <c r="H7" s="52" t="s">
+        <v>43</v>
       </c>
       <c r="I7" s="52" t="s">
         <v>167</v>
@@ -1825,8 +1843,8 @@
       <c r="G8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="53">
-        <v>2</v>
+      <c r="H8" s="53" t="s">
+        <v>43</v>
       </c>
       <c r="I8" s="53" t="s">
         <v>166</v>
@@ -1868,8 +1886,8 @@
       <c r="G9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="53">
-        <v>2</v>
+      <c r="H9" s="53" t="s">
+        <v>43</v>
       </c>
       <c r="I9" s="53" t="s">
         <v>166</v>
@@ -1923,8 +1941,8 @@
       <c r="G10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="53">
-        <v>1</v>
+      <c r="H10" s="53" t="s">
+        <v>30</v>
       </c>
       <c r="I10" s="53" t="s">
         <v>166</v>
@@ -1990,8 +2008,8 @@
       <c r="G11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="53">
-        <v>1</v>
+      <c r="H11" s="53" t="s">
+        <v>30</v>
       </c>
       <c r="I11" s="53" t="s">
         <v>166</v>
@@ -2072,8 +2090,8 @@
       <c r="G12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="53">
-        <v>1</v>
+      <c r="H12" s="53" t="s">
+        <v>30</v>
       </c>
       <c r="I12" s="53" t="s">
         <v>167</v>
@@ -2155,8 +2173,8 @@
       <c r="G13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="53">
-        <v>1</v>
+      <c r="H13" s="53" t="s">
+        <v>30</v>
       </c>
       <c r="I13" s="53" t="s">
         <v>167</v>
@@ -2214,8 +2232,8 @@
       <c r="G14" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="9">
-        <v>2</v>
+      <c r="H14" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>167</v>
@@ -2240,7 +2258,7 @@
         <v>58</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="Z14" s="2"/>
       <c r="AK14" s="2"/>
@@ -2277,8 +2295,8 @@
       <c r="G15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="9">
-        <v>2</v>
+      <c r="H15" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>167</v>
@@ -2303,10 +2321,10 @@
         <v>58</v>
       </c>
       <c r="X15" s="4" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="Z15" s="26"/>
       <c r="AK15" s="2"/>
@@ -2343,8 +2361,8 @@
       <c r="G16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="9">
-        <v>2</v>
+      <c r="H16" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>166</v>
@@ -2368,13 +2386,13 @@
       <c r="U16" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="W16" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="X16" s="18" t="s">
+      <c r="W16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y16" s="18" t="s">
+      <c r="Y16" s="4" t="s">
         <v>55</v>
       </c>
       <c r="Z16" s="26"/>
@@ -2412,8 +2430,8 @@
       <c r="G17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="9">
-        <v>2</v>
+      <c r="H17" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>166</v>
@@ -2438,7 +2456,7 @@
         <v>58</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="X17" s="4" t="s">
         <v>55</v>
@@ -2481,8 +2499,8 @@
       <c r="G18" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="9">
-        <v>1</v>
+      <c r="H18" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>166</v>
@@ -2550,8 +2568,8 @@
       <c r="G19" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="9">
-        <v>1</v>
+      <c r="H19" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>166</v>
@@ -2576,7 +2594,7 @@
         <v>57</v>
       </c>
       <c r="W19" t="s">
-        <v>103</v>
+        <v>176</v>
       </c>
       <c r="Z19" s="26"/>
       <c r="AB19" s="26"/>
@@ -2616,17 +2634,13 @@
       <c r="G20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="10">
-        <v>1</v>
+      <c r="H20" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>167</v>
       </c>
       <c r="R20" s="2"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="Z20" s="26"/>
       <c r="AB20" s="26"/>
       <c r="AC20" s="26"/>
@@ -2665,15 +2679,15 @@
       <c r="G21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="10">
-        <v>1</v>
+      <c r="H21" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>167</v>
       </c>
       <c r="R21" s="2"/>
-      <c r="X21" s="4" t="s">
-        <v>163</v>
+      <c r="W21" t="s">
+        <v>103</v>
       </c>
       <c r="Z21" s="26"/>
       <c r="AB21" s="4"/>
@@ -2713,8 +2727,8 @@
       <c r="G22" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="10">
-        <v>2</v>
+      <c r="H22" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>167</v>
@@ -2731,6 +2745,10 @@
       </c>
       <c r="T22" t="s">
         <v>138</v>
+      </c>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
@@ -2766,8 +2784,8 @@
       <c r="G23" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="10">
-        <v>2</v>
+      <c r="H23" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>167</v>
@@ -2790,6 +2808,9 @@
       </c>
       <c r="U23" t="s">
         <v>26</v>
+      </c>
+      <c r="X23" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
@@ -2825,8 +2846,8 @@
       <c r="G24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="10">
-        <v>2</v>
+      <c r="H24" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>166</v>
@@ -2884,8 +2905,8 @@
       <c r="G25" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="10">
-        <v>2</v>
+      <c r="H25" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
edit script to ask if want to see vid again
</commit_message>
<xml_diff>
--- a/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
+++ b/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1BDB49-BB26-DA40-BA8E-F72AFDD85C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2345F67-A556-594F-8ACA-66FA55DD3BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="189">
   <si>
     <t>curvilinear</t>
   </si>
@@ -3552,8 +3552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EB3C47-5A75-7B42-A854-C31509C645B3}">
   <dimension ref="A1:AU56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5432,6 +5432,9 @@
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
       <c r="G34" s="31"/>
+      <c r="I34" t="s">
+        <v>161</v>
+      </c>
       <c r="AS34" s="28"/>
     </row>
     <row r="35" spans="5:45" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added pretest event order counterbalance
</commit_message>
<xml_diff>
--- a/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
+++ b/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2345F67-A556-594F-8ACA-66FA55DD3BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69CB271-55CD-FE44-9D70-FC1F2862955C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="15" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="194">
   <si>
     <t>curvilinear</t>
   </si>
@@ -603,6 +603,21 @@
   </si>
   <si>
     <t>counterbalances whether inconsistent (rectilinear) or consistent (curvilinear) test event is shown first</t>
+  </si>
+  <si>
+    <t>PreTest Event Order Lengend</t>
+  </si>
+  <si>
+    <t>Blue (Like)</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>PreTest Event Order</t>
+  </si>
+  <si>
+    <t>counterbalances the left/right placement of the pretest events (blue/organe)</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F280014F-0359-6C4E-A6CF-E9866AFD4F4E}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1326,65 +1341,73 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>165</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3550,78 +3573,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EB3C47-5A75-7B42-A854-C31509C645B3}">
-  <dimension ref="A1:AU56"/>
+  <dimension ref="A1:AV56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="9" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" customWidth="1"/>
-    <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" customWidth="1"/>
-    <col min="27" max="27" width="8.6640625" customWidth="1"/>
-    <col min="28" max="28" width="11.33203125" customWidth="1"/>
-    <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="45" max="45" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" customWidth="1"/>
+    <col min="25" max="25" width="10.33203125" customWidth="1"/>
+    <col min="28" max="28" width="8.6640625" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" customWidth="1"/>
+    <col min="30" max="30" width="13" customWidth="1"/>
+    <col min="46" max="46" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>161</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
@@ -3629,172 +3656,178 @@
       <c r="AP1" s="2"/>
       <c r="AQ1" s="2"/>
       <c r="AR1" s="2"/>
-      <c r="AS1" s="50"/>
-      <c r="AT1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="50"/>
       <c r="AU1" s="2"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV1" s="2"/>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="52">
         <v>1</v>
       </c>
       <c r="B2" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="52">
+      <c r="D2" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="52">
         <v>1</v>
       </c>
-      <c r="E2" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="52">
+      <c r="F2" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="52">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>30</v>
+      <c r="H2" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="I2" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>169</v>
-      </c>
       <c r="M2" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="P2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="33"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
-      <c r="AS2" s="26"/>
-      <c r="AT2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="26"/>
       <c r="AU2" s="2"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV2" s="2"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="52">
         <v>2</v>
       </c>
       <c r="B3" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="52">
+      <c r="D3" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="52">
         <v>1</v>
       </c>
-      <c r="E3" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="52">
+      <c r="F3" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="52">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="L3" s="4" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="O3" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="18" t="s">
-        <v>28</v>
-      </c>
       <c r="Q3" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="X3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="X3" s="6">
+      <c r="Y3" s="6">
         <v>1</v>
       </c>
-      <c r="Y3" s="6">
-        <v>2</v>
-      </c>
       <c r="Z3" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="6">
         <v>3</v>
       </c>
-      <c r="AA3" s="6">
+      <c r="AB3" s="6">
         <v>4</v>
       </c>
-      <c r="AB3" s="6">
+      <c r="AC3" s="6">
         <v>8</v>
       </c>
-      <c r="AC3" s="6">
+      <c r="AD3" s="6">
         <v>7</v>
       </c>
-      <c r="AD3" s="6">
+      <c r="AE3" s="6">
         <v>6</v>
       </c>
-      <c r="AE3" s="6">
+      <c r="AF3" s="6">
         <v>5</v>
       </c>
-      <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
@@ -3802,254 +3835,263 @@
       <c r="AP3" s="2"/>
       <c r="AQ3" s="2"/>
       <c r="AR3" s="2"/>
-      <c r="AS3" s="26"/>
-      <c r="AT3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="26"/>
       <c r="AU3" s="2"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV3" s="2"/>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>3</v>
       </c>
       <c r="B4" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="52">
+      <c r="D4" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="52">
         <v>1</v>
       </c>
-      <c r="E4" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="52">
+      <c r="F4" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="52">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="L4" s="4" t="s">
-        <v>172</v>
+        <v>29</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="O4" t="s">
+        <v>191</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="P4" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="S4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="X4">
-        <v>2</v>
-      </c>
       <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
         <v>4</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>1</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>3</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>7</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>5</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>8</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>6</v>
       </c>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="26"/>
+      <c r="AL4" s="2"/>
       <c r="AM4" s="26"/>
-      <c r="AN4" s="2"/>
+      <c r="AN4" s="26"/>
       <c r="AO4" s="2"/>
       <c r="AP4" s="2"/>
       <c r="AQ4" s="2"/>
       <c r="AR4" s="2"/>
-      <c r="AS4" s="26"/>
-      <c r="AT4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="26"/>
       <c r="AU4" s="2"/>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV4" s="2"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>4</v>
       </c>
       <c r="B5" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="52">
+      <c r="D5" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="52">
         <v>1</v>
       </c>
-      <c r="E5" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="52">
-        <v>2</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="52" t="s">
-        <v>30</v>
+      <c r="F5" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="52">
+        <v>2</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="I5" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="18" t="s">
-        <v>30</v>
-      </c>
       <c r="Q5" s="18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="S5" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="W5" s="18" t="s">
+      <c r="T5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="X5" s="6">
+      <c r="Y5" s="6">
         <v>3</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Z5" s="6">
         <v>1</v>
       </c>
-      <c r="Z5" s="6">
+      <c r="AA5" s="6">
         <v>4</v>
       </c>
-      <c r="AA5" s="6">
-        <v>2</v>
-      </c>
       <c r="AB5" s="6">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="6">
         <v>6</v>
       </c>
-      <c r="AC5" s="6">
+      <c r="AD5" s="6">
         <v>8</v>
       </c>
-      <c r="AD5" s="6">
+      <c r="AE5" s="6">
         <v>5</v>
       </c>
-      <c r="AE5" s="6">
+      <c r="AF5" s="6">
         <v>7</v>
       </c>
-      <c r="AK5" s="2"/>
-      <c r="AL5" s="26"/>
+      <c r="AL5" s="2"/>
       <c r="AM5" s="26"/>
-      <c r="AN5" s="2"/>
+      <c r="AN5" s="26"/>
       <c r="AO5" s="2"/>
       <c r="AP5" s="2"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
-      <c r="AS5" s="26"/>
-      <c r="AT5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="26"/>
       <c r="AU5" s="2"/>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV5" s="2"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>5</v>
       </c>
       <c r="B6" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="52">
+      <c r="D6" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="52">
         <v>1</v>
       </c>
-      <c r="E6" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="52">
-        <v>2</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="52" t="s">
+      <c r="F6" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="52">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="J6" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="Q6" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="R6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W6" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X6" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>4</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>3</v>
       </c>
-      <c r="Z6">
-        <v>2</v>
-      </c>
       <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
         <v>1</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>5</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>6</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>7</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>8</v>
       </c>
-      <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
@@ -4057,44 +4099,47 @@
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
-      <c r="AS6" s="26"/>
-      <c r="AT6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="26"/>
       <c r="AU6" s="2"/>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV6" s="2"/>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>6</v>
       </c>
       <c r="B7" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="52">
+      <c r="D7" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="52">
         <v>1</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="52">
-        <v>2</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="52" t="s">
+      <c r="F7" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="52">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="52" t="s">
+      <c r="J7" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="26"/>
+      <c r="P7" s="2"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
-      <c r="S7" s="2"/>
-      <c r="AK7" s="2"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
@@ -4102,97 +4147,103 @@
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
-      <c r="AS7" s="26"/>
-      <c r="AT7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="26"/>
       <c r="AU7" s="2"/>
-    </row>
-    <row r="8" spans="1:47" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AV7" s="2"/>
+    </row>
+    <row r="8" spans="1:48" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="53">
         <v>7</v>
       </c>
       <c r="B8" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="53">
-        <v>2</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="53">
+      <c r="D8" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="53">
+        <v>2</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="53">
         <v>3</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="53" t="s">
+      <c r="H8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="J8" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="AK8" s="2"/>
-      <c r="AL8" s="33"/>
-      <c r="AM8" s="2"/>
+      <c r="S8" s="4"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="33"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
-      <c r="AS8" s="26"/>
-      <c r="AT8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="26"/>
       <c r="AU8" s="2"/>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV8" s="2"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="53">
         <v>8</v>
       </c>
       <c r="B9" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="53">
-        <v>2</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="53">
+      <c r="D9" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="53">
+        <v>2</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="53">
         <v>3</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="J9" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="O9" s="3" t="s">
+      <c r="L9" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="P9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="W9" s="3" t="s">
+      <c r="X9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AA9" s="3" t="s">
+      <c r="AB9" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
@@ -4200,67 +4251,70 @@
       <c r="AP9" s="2"/>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
-      <c r="AS9" s="26"/>
-      <c r="AT9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="26"/>
       <c r="AU9" s="2"/>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV9" s="2"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10" s="53">
         <v>9</v>
       </c>
       <c r="B10" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="53">
-        <v>2</v>
-      </c>
-      <c r="E10" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="53">
+      <c r="D10" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="53">
+        <v>2</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="53">
         <v>3</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="53" t="s">
-        <v>30</v>
+      <c r="H10" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="I10" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="L10" t="s">
-        <v>81</v>
-      </c>
-      <c r="M10" t="s">
-        <v>96</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="M10" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="P10" t="s">
         <v>142</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>126</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>143</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>126</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="Y10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AB10" s="4" t="s">
+      <c r="AC10" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="AC10" s="4" t="s">
+      <c r="AD10" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="AK10" s="2"/>
-      <c r="AL10" s="26"/>
+      <c r="AL10" s="2"/>
       <c r="AM10" s="26"/>
       <c r="AN10" s="26"/>
       <c r="AO10" s="26"/>
@@ -4268,81 +4322,84 @@
       <c r="AQ10" s="26"/>
       <c r="AR10" s="26"/>
       <c r="AS10" s="26"/>
-      <c r="AT10" s="2"/>
+      <c r="AT10" s="26"/>
       <c r="AU10" s="2"/>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV10" s="2"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11" s="53">
         <v>10</v>
       </c>
       <c r="B11" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="C11" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="53">
-        <v>2</v>
-      </c>
-      <c r="E11" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="53">
+      <c r="D11" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="53">
+        <v>2</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="53">
         <v>4</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="L11" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="P11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>25</v>
+      </c>
+      <c r="R11" t="s">
+        <v>26</v>
+      </c>
+      <c r="T11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U11" t="s">
+        <v>25</v>
+      </c>
+      <c r="V11" t="s">
+        <v>26</v>
+      </c>
+      <c r="X11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P11" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>26</v>
-      </c>
-      <c r="S11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T11" t="s">
-        <v>25</v>
-      </c>
-      <c r="U11" t="s">
-        <v>26</v>
-      </c>
-      <c r="W11" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA11" s="4" t="s">
+      <c r="AB11" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="AB11" s="4" t="s">
+      <c r="AC11" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="AC11" s="4" t="s">
+      <c r="AD11" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="26"/>
+      <c r="AL11" s="2"/>
       <c r="AM11" s="26"/>
       <c r="AN11" s="26"/>
       <c r="AO11" s="26"/>
@@ -4350,82 +4407,85 @@
       <c r="AQ11" s="26"/>
       <c r="AR11" s="26"/>
       <c r="AS11" s="26"/>
-      <c r="AT11" s="2"/>
+      <c r="AT11" s="26"/>
       <c r="AU11" s="2"/>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV11" s="2"/>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" s="53">
         <v>11</v>
       </c>
       <c r="B12" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="53">
-        <v>2</v>
-      </c>
-      <c r="E12" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="53">
+      <c r="D12" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="53">
+        <v>2</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="53">
         <v>4</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="53" t="s">
+      <c r="H12" s="8" t="s">
         <v>30</v>
       </c>
       <c r="I12" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="L12" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="R12" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="35" t="s">
+      <c r="V12" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Q12" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="R12" s="2"/>
-      <c r="S12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T12" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="U12" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA12" s="4" t="s">
+      <c r="AB12" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="AB12" s="4" t="s">
+      <c r="AC12" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AC12" s="4" t="s">
+      <c r="AD12" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="AK12" s="2"/>
-      <c r="AL12" s="26"/>
+      <c r="AL12" s="2"/>
       <c r="AM12" s="26"/>
       <c r="AN12" s="26"/>
       <c r="AO12" s="26"/>
@@ -4433,324 +4493,342 @@
       <c r="AQ12" s="26"/>
       <c r="AR12" s="26"/>
       <c r="AS12" s="26"/>
-      <c r="AT12" s="2"/>
+      <c r="AT12" s="26"/>
       <c r="AU12" s="2"/>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV12" s="2"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" s="53">
         <v>12</v>
       </c>
       <c r="B13" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="53">
-        <v>2</v>
-      </c>
-      <c r="E13" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="53">
+      <c r="D13" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="53">
+        <v>2</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="53">
         <v>4</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="53" t="s">
-        <v>30</v>
+      <c r="H13" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="I13" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="35" t="s">
+      <c r="P13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="Q13" s="35" t="s">
+      <c r="R13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="R13" s="2"/>
-      <c r="S13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T13" s="35" t="s">
+      <c r="S13" s="2"/>
+      <c r="T13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U13" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="U13" s="35" t="s">
+      <c r="V13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="26"/>
-      <c r="AM13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="26"/>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
-      <c r="AS13" s="26"/>
-      <c r="AT13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="26"/>
       <c r="AU13" s="2"/>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV13" s="2"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="D14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="9">
         <v>3</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="9">
+      <c r="F14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="9">
         <v>1</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="J14" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P14" s="37" t="s">
+      <c r="P14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Q14" s="37" t="s">
+      <c r="R14" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="R14" s="2"/>
-      <c r="S14" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="T14" s="37" t="s">
+      <c r="S14" s="2"/>
+      <c r="T14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="U14" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="U14" s="37" t="s">
+      <c r="V14" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="X14" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="Z14" s="2"/>
-      <c r="AK14" s="2"/>
+      <c r="AA14" s="2"/>
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
-      <c r="AP14" s="26"/>
+      <c r="AP14" s="2"/>
       <c r="AQ14" s="26"/>
       <c r="AR14" s="26"/>
       <c r="AS14" s="26"/>
-      <c r="AT14" s="2"/>
+      <c r="AT14" s="26"/>
       <c r="AU14" s="2"/>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV14" s="2"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="9">
+      <c r="D15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="9">
         <v>3</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="9">
+      <c r="F15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="9">
         <v>1</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="J15" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="O15" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" s="37" t="s">
+      <c r="P15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Q15" s="37" t="s">
+      <c r="R15" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="T15" s="37" t="s">
+      <c r="S15" s="2"/>
+      <c r="T15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="U15" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="U15" s="37" t="s">
+      <c r="V15" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="Y15" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="Y15" s="4" t="s">
+      <c r="Z15" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="Z15" s="26"/>
-      <c r="AK15" s="2"/>
-      <c r="AL15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AL15" s="2"/>
       <c r="AM15" s="26"/>
-      <c r="AN15" s="2"/>
+      <c r="AN15" s="26"/>
       <c r="AO15" s="2"/>
-      <c r="AP15" s="26"/>
+      <c r="AP15" s="2"/>
       <c r="AQ15" s="26"/>
       <c r="AR15" s="26"/>
       <c r="AS15" s="26"/>
-      <c r="AT15" s="2"/>
+      <c r="AT15" s="26"/>
       <c r="AU15" s="2"/>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV15" s="2"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="D16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="9">
         <v>3</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="F16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="9">
         <v>1</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="J16" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="O16" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="P16" s="36" t="s">
+      <c r="P16" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="Q16" s="36" t="s">
+      <c r="R16" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="T16" s="36" t="s">
+      <c r="S16" s="2"/>
+      <c r="T16" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="U16" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="U16" s="36" t="s">
+      <c r="V16" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="W16" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="X16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y16" s="4" t="s">
+      <c r="Z16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Z16" s="26"/>
-      <c r="AK16" s="2"/>
+      <c r="AA16" s="26"/>
       <c r="AL16" s="2"/>
-      <c r="AM16" s="26"/>
-      <c r="AN16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="26"/>
       <c r="AO16" s="2"/>
-      <c r="AP16" s="26"/>
+      <c r="AP16" s="2"/>
       <c r="AQ16" s="26"/>
       <c r="AR16" s="26"/>
       <c r="AS16" s="26"/>
-      <c r="AT16" s="2"/>
+      <c r="AT16" s="26"/>
       <c r="AU16" s="2"/>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV16" s="2"/>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="D17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="9">
         <v>3</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="9">
-        <v>2</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="9" t="s">
+      <c r="F17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="9">
+        <v>2</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="J17" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="O17" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="P17" s="36" t="s">
+      <c r="L17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q17" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="Q17" s="36" t="s">
+      <c r="R17" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="T17" s="36" t="s">
+      <c r="S17" s="2"/>
+      <c r="T17" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="U17" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="U17" s="36" t="s">
+      <c r="V17" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="W17" s="4" t="s">
+      <c r="X17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="X17" s="4" t="s">
+      <c r="Y17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Y17" s="4" t="s">
+      <c r="Z17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Z17" s="26"/>
-      <c r="AK17" s="2"/>
+      <c r="AA17" s="26"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
@@ -4758,68 +4836,74 @@
       <c r="AP17" s="2"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2"/>
-      <c r="AS17" s="26"/>
-      <c r="AT17" s="2"/>
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="26"/>
       <c r="AU17" s="2"/>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV17" s="2"/>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="9">
+      <c r="D18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="9">
         <v>3</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="9">
-        <v>2</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>30</v>
+      <c r="F18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="9">
+        <v>2</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="I18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>166</v>
       </c>
       <c r="M18" t="s">
-        <v>161</v>
-      </c>
-      <c r="O18" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="N18" t="s">
+        <v>96</v>
+      </c>
+      <c r="P18" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="P18" s="6" t="s">
+      <c r="Q18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Q18" s="6" t="s">
+      <c r="R18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="R18" s="2"/>
-      <c r="S18" s="18" t="s">
+      <c r="S18" s="2"/>
+      <c r="T18" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="U18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="U18" s="6" t="s">
+      <c r="V18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="W18" s="26"/>
       <c r="X18" s="26"/>
       <c r="Y18" s="26"/>
       <c r="Z18" s="26"/>
-      <c r="AB18" s="26"/>
+      <c r="AA18" s="26"/>
       <c r="AC18" s="26"/>
       <c r="AD18" s="26"/>
-      <c r="AK18" s="2"/>
+      <c r="AE18" s="26"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
@@ -4827,65 +4911,77 @@
       <c r="AP18" s="2"/>
       <c r="AQ18" s="2"/>
       <c r="AR18" s="2"/>
-      <c r="AS18" s="26"/>
-      <c r="AT18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="26"/>
       <c r="AU18" s="2"/>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV18" s="2"/>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="9">
+      <c r="D19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="9">
         <v>3</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="9">
-        <v>2</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="9" t="s">
+      <c r="F19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="9">
+        <v>2</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="O19" s="18" t="s">
+      <c r="L19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P19" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="P19" s="6" t="s">
+      <c r="Q19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Q19" s="6" t="s">
+      <c r="R19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="2"/>
-      <c r="S19" s="18" t="s">
+      <c r="S19" s="2"/>
+      <c r="T19" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="U19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="U19" s="6" t="s">
+      <c r="V19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>176</v>
       </c>
-      <c r="Z19" s="26"/>
-      <c r="AB19" s="26"/>
+      <c r="AA19" s="26"/>
       <c r="AC19" s="26"/>
       <c r="AD19" s="26"/>
-      <c r="AK19" s="2"/>
+      <c r="AE19" s="26"/>
       <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
@@ -4893,44 +4989,56 @@
       <c r="AP19" s="2"/>
       <c r="AQ19" s="2"/>
       <c r="AR19" s="2"/>
-      <c r="AS19" s="26"/>
-      <c r="AT19" s="2"/>
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="26"/>
       <c r="AU19" s="2"/>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV19" s="2"/>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="10">
+      <c r="D20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="10">
         <v>4</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="10">
+      <c r="F20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="10">
         <v>3</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="13" t="s">
         <v>30</v>
       </c>
       <c r="I20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="R20" s="2"/>
-      <c r="Z20" s="26"/>
-      <c r="AB20" s="26"/>
+      <c r="L20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="2"/>
+      <c r="AA20" s="26"/>
       <c r="AC20" s="26"/>
       <c r="AD20" s="26"/>
-      <c r="AK20" s="2"/>
+      <c r="AE20" s="26"/>
       <c r="AL20" s="2"/>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
@@ -4938,47 +5046,50 @@
       <c r="AP20" s="2"/>
       <c r="AQ20" s="2"/>
       <c r="AR20" s="2"/>
-      <c r="AS20" s="26"/>
-      <c r="AT20" s="2"/>
+      <c r="AS20" s="2"/>
+      <c r="AT20" s="26"/>
       <c r="AU20" s="2"/>
-    </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV20" s="2"/>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="10">
+      <c r="D21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="10">
         <v>4</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="10">
+      <c r="F21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="10">
         <v>3</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>30</v>
+      <c r="H21" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="I21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="R21" s="2"/>
-      <c r="W21" t="s">
+      <c r="S21" s="2"/>
+      <c r="X21" t="s">
         <v>103</v>
       </c>
-      <c r="Z21" s="26"/>
-      <c r="AB21" s="4"/>
+      <c r="AA21" s="26"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
-      <c r="AK21" s="2"/>
+      <c r="AE21" s="4"/>
       <c r="AL21" s="2"/>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
@@ -4986,56 +5097,59 @@
       <c r="AP21" s="2"/>
       <c r="AQ21" s="2"/>
       <c r="AR21" s="2"/>
-      <c r="AS21" s="26"/>
-      <c r="AT21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="26"/>
       <c r="AU21" s="2"/>
-    </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV21" s="2"/>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="10">
+      <c r="D22" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="10">
         <v>4</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="10">
+      <c r="F22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="10">
         <v>3</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="J22" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>142</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>138</v>
       </c>
-      <c r="R22" s="2"/>
-      <c r="S22" t="s">
+      <c r="S22" s="2"/>
+      <c r="T22" t="s">
         <v>143</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>138</v>
       </c>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4" t="s">
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
@@ -5043,61 +5157,64 @@
       <c r="AP22" s="2"/>
       <c r="AQ22" s="2"/>
       <c r="AR22" s="2"/>
-      <c r="AS22" s="26"/>
-      <c r="AT22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="26"/>
       <c r="AU22" s="2"/>
-    </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV22" s="2"/>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="10">
+      <c r="D23" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="10">
         <v>4</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="10">
+      <c r="F23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="10">
         <v>4</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="J23" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>27</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>25</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>26</v>
       </c>
-      <c r="R23" s="2"/>
-      <c r="S23" t="s">
+      <c r="S23" s="2"/>
+      <c r="T23" t="s">
         <v>27</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>25</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>26</v>
       </c>
-      <c r="X23" s="4" t="s">
+      <c r="Y23" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
@@ -5105,58 +5222,61 @@
       <c r="AP23" s="2"/>
       <c r="AQ23" s="2"/>
       <c r="AR23" s="2"/>
-      <c r="AS23" s="26"/>
-      <c r="AT23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="26"/>
       <c r="AU23" s="2"/>
-    </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV23" s="2"/>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="D24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="10">
         <v>4</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="10">
+      <c r="F24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="10">
         <v>4</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="J24" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P24" s="35" t="s">
+      <c r="P24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="Q24" s="35" t="s">
+      <c r="R24" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="R24" s="2"/>
-      <c r="S24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T24" s="35" t="s">
+      <c r="S24" s="2"/>
+      <c r="T24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U24" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="U24" s="35" t="s">
+      <c r="V24" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
@@ -5164,58 +5284,61 @@
       <c r="AP24" s="2"/>
       <c r="AQ24" s="2"/>
       <c r="AR24" s="2"/>
-      <c r="AS24" s="26"/>
-      <c r="AT24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="26"/>
       <c r="AU24" s="2"/>
-    </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV24" s="2"/>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="10">
+      <c r="D25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="10">
         <v>4</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="10">
+      <c r="F25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="10">
         <v>4</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="J25" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P25" s="35" t="s">
+      <c r="P25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="Q25" s="35" t="s">
+      <c r="R25" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="R25" s="2"/>
-      <c r="S25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T25" s="35" t="s">
+      <c r="S25" s="2"/>
+      <c r="T25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U25" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="U25" s="35" t="s">
+      <c r="V25" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
@@ -5223,31 +5346,31 @@
       <c r="AP25" s="2"/>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
-      <c r="AS25" s="26"/>
-      <c r="AT25" s="2"/>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="26"/>
       <c r="AU25" s="2"/>
-    </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="O26" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26" s="37" t="s">
+      <c r="AV25" s="2"/>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="P26" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q26" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Q26" s="37" t="s">
+      <c r="R26" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="R26" s="2"/>
-      <c r="S26" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="T26" s="37" t="s">
+      <c r="S26" s="2"/>
+      <c r="T26" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="U26" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="U26" s="37" t="s">
+      <c r="V26" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="AK26" s="2"/>
       <c r="AL26" s="2"/>
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
@@ -5258,35 +5381,37 @@
       <c r="AS26" s="2"/>
       <c r="AT26" s="2"/>
       <c r="AU26" s="2"/>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV26" s="2"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="26"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="26"/>
-      <c r="O27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27" s="37" t="s">
+      <c r="J27" s="26"/>
+      <c r="P27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q27" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Q27" s="37" t="s">
+      <c r="R27" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="R27" s="2"/>
-      <c r="S27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="T27" s="37" t="s">
+      <c r="S27" s="2"/>
+      <c r="T27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="U27" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="U27" s="37" t="s">
+      <c r="V27" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="AK27" s="2"/>
       <c r="AL27" s="2"/>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
@@ -5297,35 +5422,37 @@
       <c r="AS27" s="2"/>
       <c r="AT27" s="2"/>
       <c r="AU27" s="2"/>
-    </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="C28" s="2"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="2"/>
-      <c r="O28" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="P28" s="36" t="s">
+      <c r="AV27" s="2"/>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="P28" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="Q28" s="36" t="s">
+      <c r="R28" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="2"/>
-      <c r="S28" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="T28" s="36" t="s">
+      <c r="S28" s="2"/>
+      <c r="T28" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="U28" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="U28" s="36" t="s">
+      <c r="V28" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="AK28" s="2"/>
       <c r="AL28" s="2"/>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
@@ -5336,8 +5463,10 @@
       <c r="AS28" s="2"/>
       <c r="AT28" s="2"/>
       <c r="AU28" s="2"/>
-    </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AV28" s="2"/>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -5345,218 +5474,246 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="O29" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="P29" s="36" t="s">
+      <c r="J29" s="2"/>
+      <c r="P29" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="Q29" s="36" t="s">
+      <c r="R29" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="R29" s="2"/>
-      <c r="S29" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="T29" s="36" t="s">
+      <c r="S29" s="2"/>
+      <c r="T29" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="U29" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="U29" s="36" t="s">
+      <c r="V29" s="36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="O30" s="18" t="s">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="P30" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="P30" s="6" t="s">
+      <c r="Q30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="R30" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="R30" s="2"/>
-      <c r="S30" s="18" t="s">
+      <c r="S30" s="2"/>
+      <c r="T30" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="T30" s="6" t="s">
+      <c r="U30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="U30" s="6" t="s">
+      <c r="V30" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AS30" s="5"/>
-    </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="O31" s="18" t="s">
+      <c r="AT30" s="5"/>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="P31" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="P31" s="6" t="s">
+      <c r="Q31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Q31" s="6" t="s">
+      <c r="R31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="R31" s="2"/>
-      <c r="S31" s="18" t="s">
+      <c r="S31" s="2"/>
+      <c r="T31" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="T31" s="6" t="s">
+      <c r="U31" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="U31" s="6" t="s">
+      <c r="V31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AS31" s="27"/>
-    </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="28"/>
-      <c r="R32" s="2"/>
-      <c r="AS32" s="28"/>
-    </row>
-    <row r="33" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="31"/>
-      <c r="AS33" s="28"/>
-    </row>
-    <row r="34" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="31"/>
-      <c r="I34" t="s">
-        <v>161</v>
-      </c>
-      <c r="AS34" s="28"/>
-    </row>
-    <row r="35" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E35" s="29"/>
+      <c r="AT31" s="27"/>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="AT32" s="28"/>
+    </row>
+    <row r="33" spans="2:46" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="AT33" s="28"/>
+    </row>
+    <row r="34" spans="2:46" x14ac:dyDescent="0.2">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="AT34" s="28"/>
+    </row>
+    <row r="35" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F35" s="29"/>
-      <c r="G35" s="31"/>
-      <c r="AS35" s="28"/>
-    </row>
-    <row r="36" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E36" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="31"/>
+      <c r="AT35" s="28"/>
+    </row>
+    <row r="36" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F36" s="29"/>
-      <c r="G36" s="28"/>
-      <c r="AS36" s="28"/>
-    </row>
-    <row r="37" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E37" s="4"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="28"/>
+      <c r="AT36" s="28"/>
+    </row>
+    <row r="37" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="AS37" s="4"/>
-    </row>
-    <row r="38" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E38" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="AT37" s="4"/>
+    </row>
+    <row r="38" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="AS38" s="4"/>
-    </row>
-    <row r="39" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E39" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="AT38" s="4"/>
+    </row>
+    <row r="39" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F39" s="4"/>
-      <c r="G39" s="26"/>
-      <c r="AS39" s="4"/>
-    </row>
-    <row r="40" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="G40" s="33"/>
-      <c r="AS40" s="3"/>
-    </row>
-    <row r="41" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E41" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="26"/>
+      <c r="AT39" s="4"/>
+    </row>
+    <row r="40" spans="2:46" x14ac:dyDescent="0.2">
+      <c r="H40" s="33"/>
+      <c r="AT40" s="3"/>
+    </row>
+    <row r="41" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F41" s="4"/>
-      <c r="G41" s="34"/>
-      <c r="AS41" s="19"/>
-    </row>
-    <row r="42" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E42" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="34"/>
+      <c r="AT41" s="19"/>
+    </row>
+    <row r="42" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F42" s="4"/>
-      <c r="G42" s="34"/>
-      <c r="AS42" s="19"/>
-    </row>
-    <row r="43" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E43" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="34"/>
+      <c r="AT42" s="19"/>
+    </row>
+    <row r="43" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F43" s="4"/>
-      <c r="G43" s="34"/>
-      <c r="AS43" s="19"/>
-    </row>
-    <row r="44" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E44" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="34"/>
+      <c r="AT43" s="19"/>
+    </row>
+    <row r="44" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F44" s="4"/>
-      <c r="G44" s="34"/>
-      <c r="AS44" s="19"/>
-    </row>
-    <row r="45" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E45" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="34"/>
+      <c r="AT44" s="19"/>
+    </row>
+    <row r="45" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F45" s="4"/>
-      <c r="G45" s="34"/>
-      <c r="AS45" s="19"/>
-    </row>
-    <row r="46" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E46" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="34"/>
+      <c r="AT45" s="19"/>
+    </row>
+    <row r="46" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F46" s="4"/>
-      <c r="G46" s="34"/>
-      <c r="AS46" s="19"/>
-    </row>
-    <row r="47" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E47" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="34"/>
+      <c r="AT46" s="19"/>
+    </row>
+    <row r="47" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F47" s="4"/>
-      <c r="G47" s="34"/>
-      <c r="AS47" s="19"/>
-    </row>
-    <row r="48" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E48" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="34"/>
+      <c r="AT47" s="19"/>
+    </row>
+    <row r="48" spans="2:46" x14ac:dyDescent="0.2">
       <c r="F48" s="4"/>
-      <c r="G48" s="34"/>
-      <c r="AS48" s="19"/>
-    </row>
-    <row r="49" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E49" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="34"/>
+      <c r="AT48" s="19"/>
+    </row>
+    <row r="49" spans="6:46" x14ac:dyDescent="0.2">
       <c r="F49" s="4"/>
-      <c r="G49" s="34"/>
-      <c r="AS49" s="19"/>
-    </row>
-    <row r="50" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E50" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="34"/>
+      <c r="AT49" s="19"/>
+    </row>
+    <row r="50" spans="6:46" x14ac:dyDescent="0.2">
       <c r="F50" s="4"/>
-      <c r="G50" s="34"/>
-      <c r="AS50" s="19"/>
-    </row>
-    <row r="51" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E51" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="34"/>
+      <c r="AT50" s="19"/>
+    </row>
+    <row r="51" spans="6:46" x14ac:dyDescent="0.2">
       <c r="F51" s="4"/>
-      <c r="G51" s="34"/>
-      <c r="AS51" s="19"/>
-    </row>
-    <row r="52" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E52" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="34"/>
+      <c r="AT51" s="19"/>
+    </row>
+    <row r="52" spans="6:46" x14ac:dyDescent="0.2">
       <c r="F52" s="4"/>
-      <c r="G52" s="34"/>
-      <c r="AS52" s="19"/>
-    </row>
-    <row r="53" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="E53" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="34"/>
+      <c r="AT52" s="19"/>
+    </row>
+    <row r="53" spans="6:46" x14ac:dyDescent="0.2">
       <c r="F53" s="4"/>
-      <c r="G53" s="34"/>
-      <c r="AS53" s="19"/>
-    </row>
-    <row r="54" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="5:45" x14ac:dyDescent="0.2">
-      <c r="G56" s="2"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="34"/>
+      <c r="AT53" s="19"/>
+    </row>
+    <row r="54" spans="6:46" x14ac:dyDescent="0.2">
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="6:46" x14ac:dyDescent="0.2">
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="6:46" x14ac:dyDescent="0.2">
+      <c r="H56" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
changed test Q phrasing
</commit_message>
<xml_diff>
--- a/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
+++ b/CMCM Lab Associative Learning Study Counterbalacing (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69CB271-55CD-FE44-9D70-FC1F2862955C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402C823D-6F1C-4243-8E24-B6BF0423E1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{417284C1-A0D2-4539-9F2E-FC16F8FBD9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="15" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F280014F-0359-6C4E-A6CF-E9866AFD4F4E}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+    <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3575,8 +3575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EB3C47-5A75-7B42-A854-C31509C645B3}">
   <dimension ref="A1:AV56"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>